<commit_message>
fix(helper) : changer la couleur du texte
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -5,18 +5,18 @@
   <workbookPr updateLinks="never" codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Poo\P_oo-Shoot-me-up\doc\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb17shq\Documents\Shootmeup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B98B29A4-90F0-4BF0-A216-075B86970160}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C29B0F-26DB-4F7D-81D4-177AF2321011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$72</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$73</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -275,6 +275,42 @@
   </si>
   <si>
     <t>mouvement des projectile</t>
+  </si>
+  <si>
+    <t>Recréé un compte github</t>
+  </si>
+  <si>
+    <t>GITHUB</t>
+  </si>
+  <si>
+    <t>Ennemis</t>
+  </si>
+  <si>
+    <t>affichage</t>
+  </si>
+  <si>
+    <t>Tire des ennemis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">clic souris </t>
+  </si>
+  <si>
+    <t>tire du joueur au clic souris</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rotation du gent </t>
+  </si>
+  <si>
+    <t>Projectils</t>
+  </si>
+  <si>
+    <t>Doc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">doc de colison </t>
+  </si>
+  <si>
+    <t>https://happycoding.io/tutorials/processing/collision-detection</t>
   </si>
 </sst>
 </file>
@@ -619,18 +655,6 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -660,6 +684,18 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -976,13 +1012,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:F76"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D21" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E34" sqref="E34"/>
+      <selection pane="bottomRight" activeCell="D46" activeCellId="1" sqref="D50 D45:D46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1001,10 +1037,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="40" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="32"/>
+      <c r="C1" s="40"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -1016,10 +1052,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="32" t="s">
+      <c r="B2" s="40" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="32"/>
+      <c r="C2" s="40"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1031,10 +1067,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="32" t="s">
+      <c r="B3" s="40" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="32"/>
+      <c r="C3" s="40"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -1046,12 +1082,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="33" t="s">
+      <c r="B4" s="41" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="34"/>
-      <c r="D4" s="34"/>
-      <c r="E4" s="35"/>
+      <c r="C4" s="42"/>
+      <c r="D4" s="42"/>
+      <c r="E4" s="43"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1074,7 +1110,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="36">
+      <c r="B6" s="32">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -1089,7 +1125,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="37"/>
+      <c r="B7" s="33"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -1102,7 +1138,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="33"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1115,14 +1151,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="37"/>
+      <c r="B9" s="33"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="38"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1131,16 +1167,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="39"/>
-      <c r="C11" s="40"/>
-      <c r="D11" s="40"/>
-      <c r="E11" s="41"/>
+      <c r="B11" s="35"/>
+      <c r="C11" s="36"/>
+      <c r="D11" s="36"/>
+      <c r="E11" s="37"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="36">
+      <c r="B12" s="32">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1156,7 +1192,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="37"/>
+      <c r="B13" s="33"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1169,7 +1205,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="37"/>
+      <c r="B14" s="33"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1185,7 +1221,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="33"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1200,7 +1236,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="37"/>
+      <c r="B16" s="33"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1213,7 +1249,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="37"/>
+      <c r="B17" s="33"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1224,7 +1260,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="38"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1233,16 +1269,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="39"/>
-      <c r="C19" s="40"/>
-      <c r="D19" s="40"/>
-      <c r="E19" s="41"/>
+      <c r="B19" s="35"/>
+      <c r="C19" s="36"/>
+      <c r="D19" s="36"/>
+      <c r="E19" s="37"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="36">
+      <c r="B20" s="32">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1257,7 +1293,7 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="37"/>
+      <c r="B21" s="33"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1269,7 +1305,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="37"/>
+      <c r="B22" s="33"/>
       <c r="C22" s="8">
         <v>20</v>
       </c>
@@ -1281,7 +1317,7 @@
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="37"/>
+      <c r="B23" s="33"/>
       <c r="C23" s="8">
         <v>30</v>
       </c>
@@ -1293,7 +1329,7 @@
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="38"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="10">
         <v>60</v>
       </c>
@@ -1305,16 +1341,16 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="39"/>
-      <c r="C25" s="40"/>
-      <c r="D25" s="40"/>
-      <c r="E25" s="41"/>
+      <c r="B25" s="35"/>
+      <c r="C25" s="36"/>
+      <c r="D25" s="36"/>
+      <c r="E25" s="37"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="36">
+      <c r="B26" s="32">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1332,7 +1368,7 @@
       <c r="A27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="37"/>
+      <c r="B27" s="33"/>
       <c r="C27" s="27">
         <v>20</v>
       </c>
@@ -1344,7 +1380,7 @@
       <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="37"/>
+      <c r="B28" s="33"/>
       <c r="C28" s="27">
         <v>20</v>
       </c>
@@ -1356,7 +1392,7 @@
       <c r="A29" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="37"/>
+      <c r="B29" s="33"/>
       <c r="C29" s="27">
         <v>20</v>
       </c>
@@ -1368,7 +1404,7 @@
       <c r="A30" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="37"/>
+      <c r="B30" s="33"/>
       <c r="C30" s="27">
         <v>20</v>
       </c>
@@ -1380,7 +1416,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="37"/>
+      <c r="B31" s="33"/>
       <c r="C31" s="27">
         <v>10</v>
       </c>
@@ -1392,7 +1428,7 @@
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="38"/>
+      <c r="B32" s="34"/>
       <c r="C32" s="27">
         <v>10</v>
       </c>
@@ -1405,16 +1441,16 @@
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="39"/>
-      <c r="C33" s="40"/>
-      <c r="D33" s="40"/>
-      <c r="E33" s="41"/>
+      <c r="B33" s="35"/>
+      <c r="C33" s="36"/>
+      <c r="D33" s="36"/>
+      <c r="E33" s="37"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="36">
+      <c r="B34" s="32">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1429,7 +1465,7 @@
       <c r="A35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="37"/>
+      <c r="B35" s="33"/>
       <c r="C35" s="27">
         <v>15</v>
       </c>
@@ -1441,7 +1477,7 @@
       <c r="A36" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="37"/>
+      <c r="B36" s="33"/>
       <c r="C36" s="27">
         <v>15</v>
       </c>
@@ -1454,7 +1490,7 @@
       <c r="A37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="37"/>
+      <c r="B37" s="33"/>
       <c r="C37" s="27">
         <v>30</v>
       </c>
@@ -1467,7 +1503,7 @@
       <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="37"/>
+      <c r="B38" s="33"/>
       <c r="C38" s="27">
         <v>30</v>
       </c>
@@ -1480,7 +1516,7 @@
       <c r="A39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="37"/>
+      <c r="B39" s="33"/>
       <c r="C39" s="27">
         <v>15</v>
       </c>
@@ -1493,7 +1529,7 @@
       <c r="A40" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="38"/>
+      <c r="B40" s="34"/>
       <c r="C40" s="27">
         <v>15</v>
       </c>
@@ -1503,283 +1539,319 @@
       <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="39"/>
-      <c r="C41" s="40"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="41"/>
+      <c r="B41" s="35"/>
+      <c r="C41" s="36"/>
+      <c r="D41" s="36"/>
+      <c r="E41" s="37"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="4"/>
-      <c r="B42" s="36">
+      <c r="A42" s="4" t="s">
+        <v>76</v>
+      </c>
+      <c r="B42" s="32">
         <f>B34+7</f>
         <v>45931</v>
       </c>
-      <c r="C42" s="5"/>
-      <c r="D42" s="6"/>
+      <c r="C42" s="5">
+        <v>5</v>
+      </c>
+      <c r="D42" s="6" t="s">
+        <v>75</v>
+      </c>
       <c r="E42" s="5"/>
     </row>
     <row r="43" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A43" s="7"/>
-      <c r="B43" s="37"/>
-      <c r="C43" s="8"/>
-      <c r="D43" s="9"/>
+      <c r="A43" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B43" s="33"/>
+      <c r="C43" s="8">
+        <v>40</v>
+      </c>
+      <c r="D43" s="9" t="s">
+        <v>78</v>
+      </c>
       <c r="E43" s="8"/>
     </row>
     <row r="44" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A44" s="7"/>
-      <c r="B44" s="37"/>
-      <c r="C44" s="8"/>
-      <c r="D44" s="9"/>
+      <c r="A44" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="B44" s="33"/>
+      <c r="C44" s="8">
+        <v>45</v>
+      </c>
+      <c r="D44" s="9" t="s">
+        <v>79</v>
+      </c>
       <c r="E44" s="8"/>
     </row>
     <row r="45" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A45" s="7"/>
-      <c r="B45" s="37"/>
-      <c r="C45" s="8"/>
-      <c r="D45" s="9"/>
+      <c r="A45" s="7" t="s">
+        <v>80</v>
+      </c>
+      <c r="B45" s="33"/>
+      <c r="C45" s="8">
+        <v>40</v>
+      </c>
+      <c r="D45" s="9" t="s">
+        <v>81</v>
+      </c>
       <c r="E45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="10"/>
-      <c r="B46" s="38"/>
-      <c r="C46" s="10"/>
-      <c r="D46" s="11"/>
-      <c r="E46" s="10"/>
+    <row r="46" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A46" s="23" t="s">
+        <v>84</v>
+      </c>
+      <c r="B46" s="33"/>
+      <c r="C46" s="10">
+        <v>20</v>
+      </c>
+      <c r="D46" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="47" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A47" s="12" t="s">
+      <c r="A47" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B47" s="34"/>
+      <c r="C47" s="10">
+        <v>30</v>
+      </c>
+      <c r="D47" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="E47" s="10"/>
+    </row>
+    <row r="48" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B47" s="39"/>
-      <c r="C47" s="40"/>
-      <c r="D47" s="40"/>
-      <c r="E47" s="41"/>
-    </row>
-    <row r="48" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A48" s="4"/>
-      <c r="B48" s="36">
+      <c r="B48" s="35"/>
+      <c r="C48" s="36"/>
+      <c r="D48" s="36"/>
+      <c r="E48" s="37"/>
+    </row>
+    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A49" s="4"/>
+      <c r="B49" s="32">
         <f>B42+7</f>
         <v>45938</v>
       </c>
-      <c r="C48" s="5"/>
-      <c r="D48" s="6"/>
-      <c r="E48" s="5"/>
-    </row>
-    <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="7"/>
-      <c r="B49" s="37"/>
-      <c r="C49" s="8"/>
-      <c r="D49" s="9"/>
-      <c r="E49" s="8"/>
+      <c r="C49" s="5"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A50" s="7"/>
-      <c r="B50" s="37"/>
+      <c r="B50" s="33"/>
       <c r="C50" s="8"/>
       <c r="D50" s="9"/>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A51" s="7"/>
-      <c r="B51" s="37"/>
+      <c r="B51" s="33"/>
       <c r="C51" s="8"/>
       <c r="D51" s="9"/>
       <c r="E51" s="8"/>
     </row>
-    <row r="52" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A52" s="10"/>
-      <c r="B52" s="38"/>
-      <c r="C52" s="10"/>
-      <c r="D52" s="11"/>
-      <c r="E52" s="10"/>
+    <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A52" s="7"/>
+      <c r="B52" s="33"/>
+      <c r="C52" s="8"/>
+      <c r="D52" s="9"/>
+      <c r="E52" s="8"/>
     </row>
     <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="12" t="s">
+      <c r="A53" s="10"/>
+      <c r="B53" s="34"/>
+      <c r="C53" s="10"/>
+      <c r="D53" s="11"/>
+      <c r="E53" s="10"/>
+    </row>
+    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A54" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B53" s="39"/>
-      <c r="C53" s="40"/>
-      <c r="D53" s="40"/>
-      <c r="E53" s="41"/>
-    </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="4"/>
-      <c r="B54" s="36">
-        <f>B48+7</f>
+      <c r="B54" s="35"/>
+      <c r="C54" s="36"/>
+      <c r="D54" s="36"/>
+      <c r="E54" s="37"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A55" s="4"/>
+      <c r="B55" s="32">
+        <f>B49+7</f>
         <v>45945</v>
       </c>
-      <c r="C54" s="5"/>
-      <c r="D54" s="6"/>
-      <c r="E54" s="5"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="7"/>
-      <c r="B55" s="37"/>
-      <c r="C55" s="8"/>
-      <c r="D55" s="9"/>
-      <c r="E55" s="8"/>
+      <c r="C55" s="5"/>
+      <c r="D55" s="6"/>
+      <c r="E55" s="5"/>
     </row>
     <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A56" s="7"/>
-      <c r="B56" s="37"/>
+      <c r="B56" s="33"/>
       <c r="C56" s="8"/>
       <c r="D56" s="9"/>
       <c r="E56" s="8"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="7"/>
-      <c r="B57" s="37"/>
+      <c r="B57" s="33"/>
       <c r="C57" s="8"/>
       <c r="D57" s="9"/>
       <c r="E57" s="8"/>
     </row>
-    <row r="58" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A58" s="10"/>
-      <c r="B58" s="38"/>
-      <c r="C58" s="10"/>
-      <c r="D58" s="11"/>
-      <c r="E58" s="10"/>
+    <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A58" s="7"/>
+      <c r="B58" s="33"/>
+      <c r="C58" s="8"/>
+      <c r="D58" s="9"/>
+      <c r="E58" s="8"/>
     </row>
     <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="12" t="s">
+      <c r="A59" s="10"/>
+      <c r="B59" s="34"/>
+      <c r="C59" s="10"/>
+      <c r="D59" s="11"/>
+      <c r="E59" s="10"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A60" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B59" s="39"/>
-      <c r="C59" s="40"/>
-      <c r="D59" s="40"/>
-      <c r="E59" s="41"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="4"/>
-      <c r="B60" s="36">
-        <f>B54+7</f>
+      <c r="B60" s="35"/>
+      <c r="C60" s="36"/>
+      <c r="D60" s="36"/>
+      <c r="E60" s="37"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A61" s="4"/>
+      <c r="B61" s="32">
+        <f>B55+7</f>
         <v>45952</v>
       </c>
-      <c r="C60" s="5"/>
-      <c r="D60" s="6"/>
-      <c r="E60" s="5"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="7"/>
-      <c r="B61" s="37"/>
-      <c r="C61" s="8"/>
-      <c r="D61" s="9"/>
-      <c r="E61" s="8"/>
+      <c r="C61" s="5"/>
+      <c r="D61" s="6"/>
+      <c r="E61" s="5"/>
     </row>
     <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A62" s="7"/>
-      <c r="B62" s="37"/>
+      <c r="B62" s="33"/>
       <c r="C62" s="8"/>
       <c r="D62" s="9"/>
       <c r="E62" s="8"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="7"/>
-      <c r="B63" s="37"/>
+      <c r="B63" s="33"/>
       <c r="C63" s="8"/>
       <c r="D63" s="9"/>
       <c r="E63" s="8"/>
     </row>
-    <row r="64" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A64" s="10"/>
-      <c r="B64" s="38"/>
-      <c r="C64" s="10"/>
-      <c r="D64" s="11"/>
-      <c r="E64" s="10"/>
+    <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="7"/>
+      <c r="B64" s="33"/>
+      <c r="C64" s="8"/>
+      <c r="D64" s="9"/>
+      <c r="E64" s="8"/>
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="12" t="s">
+      <c r="A65" s="10"/>
+      <c r="B65" s="34"/>
+      <c r="C65" s="10"/>
+      <c r="D65" s="11"/>
+      <c r="E65" s="10"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A66" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B65" s="39"/>
-      <c r="C65" s="40"/>
-      <c r="D65" s="40"/>
-      <c r="E65" s="41"/>
-    </row>
-    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="13"/>
-      <c r="B66" s="36">
-        <f>B60+7</f>
+      <c r="B66" s="35"/>
+      <c r="C66" s="36"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="37"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="13"/>
+      <c r="B67" s="32">
+        <f>B61+7</f>
         <v>45959</v>
       </c>
-      <c r="C66" s="13"/>
-      <c r="D66" s="14"/>
-      <c r="E66" s="13"/>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="8"/>
-      <c r="B67" s="37"/>
-      <c r="C67" s="8"/>
-      <c r="D67" s="9"/>
-      <c r="E67" s="8"/>
+      <c r="C67" s="13"/>
+      <c r="D67" s="14"/>
+      <c r="E67" s="13"/>
     </row>
     <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A68" s="8"/>
-      <c r="B68" s="37"/>
+      <c r="B68" s="33"/>
       <c r="C68" s="8"/>
       <c r="D68" s="9"/>
       <c r="E68" s="8"/>
     </row>
     <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="8"/>
-      <c r="B69" s="37"/>
+      <c r="B69" s="33"/>
       <c r="C69" s="8"/>
       <c r="D69" s="9"/>
       <c r="E69" s="8"/>
     </row>
-    <row r="70" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
-      <c r="B70" s="38"/>
+      <c r="B70" s="33"/>
       <c r="C70" s="8"/>
       <c r="D70" s="9"/>
       <c r="E70" s="8"/>
     </row>
     <row r="71" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A71" s="12" t="s">
+      <c r="A71" s="8"/>
+      <c r="B71" s="34"/>
+      <c r="C71" s="8"/>
+      <c r="D71" s="9"/>
+      <c r="E71" s="8"/>
+    </row>
+    <row r="72" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A72" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B71" s="39"/>
-      <c r="C71" s="40"/>
-      <c r="D71" s="40"/>
-      <c r="E71" s="41"/>
-    </row>
-    <row r="72" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="42" t="s">
+      <c r="B72" s="35"/>
+      <c r="C72" s="36"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="37"/>
+    </row>
+    <row r="73" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="38" t="s">
         <v>15</v>
       </c>
-      <c r="B72" s="43"/>
-      <c r="C72" s="15">
-        <f>MROUND(SUM(C6:C71) /60,0.2)</f>
-        <v>14.600000000000001</v>
-      </c>
-      <c r="D72" s="16"/>
-      <c r="E72" s="17"/>
-    </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A74" s="18" t="s">
+      <c r="B73" s="39"/>
+      <c r="C73" s="15">
+        <f>MROUND(SUM(C6:C72) /60,0.2)</f>
+        <v>17.600000000000001</v>
+      </c>
+      <c r="D73" s="16"/>
+      <c r="E73" s="17"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A75" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="18"/>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A76" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
-    <mergeCell ref="B42:B46"/>
-    <mergeCell ref="B71:E71"/>
-    <mergeCell ref="A72:B72"/>
-    <mergeCell ref="B48:B52"/>
-    <mergeCell ref="B53:E53"/>
-    <mergeCell ref="B54:B58"/>
-    <mergeCell ref="B59:E59"/>
-    <mergeCell ref="B60:B64"/>
-    <mergeCell ref="B65:E65"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B66:B70"/>
-    <mergeCell ref="B47:E47"/>
+    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B48:E48"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
     <mergeCell ref="B12:B18"/>
@@ -1790,12 +1862,21 @@
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:B40"/>
     <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B72:E72"/>
+    <mergeCell ref="A73:B73"/>
+    <mergeCell ref="B49:B53"/>
+    <mergeCell ref="B54:E54"/>
+    <mergeCell ref="B55:B59"/>
+    <mergeCell ref="B60:E60"/>
+    <mergeCell ref="B61:B65"/>
+    <mergeCell ref="B66:E66"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C60:C64 C54:C58 C42:C46 C48:C52 C20:C24 B6 C12:C18 C66:C70 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C61:C65 C55:C59 C42:C47 C49:C53 C20:C24 B6 C12:C18 C67:C71 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B60:B64 B20:B24 B26:B32 B34:B40 B42:B46 B48:B52 B54:B58 B66:B70" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B61:B65 B20:B24 B26:B32 B34:B40 B42:B47 B49:B53 B55:B59 B67:B71" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1820,6 +1901,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2062,15 +2152,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2083,6 +2164,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2101,14 +2190,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Chore(renoamge) : nomage de projectil
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,15 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb17shq\Documents\Shootmeup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6C29B0F-26DB-4F7D-81D4-177AF2321011}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{72B18A7A-F550-4644-B8FA-7EFD05DD02DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="16440" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Journal" sheetId="18" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$73</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Journal!$A$1:$E$75</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="87">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="116" uniqueCount="98">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -311,6 +311,39 @@
   </si>
   <si>
     <t>https://happycoding.io/tutorials/processing/collision-detection</t>
+  </si>
+  <si>
+    <t>Renomage</t>
+  </si>
+  <si>
+    <t>Image</t>
+  </si>
+  <si>
+    <t>Gitignore</t>
+  </si>
+  <si>
+    <t>varibale/function</t>
+  </si>
+  <si>
+    <t xml:space="preserve">passer des chemain local au </t>
+  </si>
+  <si>
+    <t>Aide Killan</t>
+  </si>
+  <si>
+    <t>Pour ses hidebox</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Affichage du socre</t>
+  </si>
+  <si>
+    <t>contoure des obstacles</t>
+  </si>
+  <si>
+    <t>differancier les projectils ennemis et non ennemis</t>
   </si>
 </sst>
 </file>
@@ -655,6 +688,18 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
@@ -684,18 +729,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1012,13 +1045,13 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:F76"/>
+  <dimension ref="A1:F78"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D25" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D38" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D46" activeCellId="1" sqref="D50 D45:D46"/>
+      <selection pane="bottomRight" activeCell="A53" sqref="A53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1037,10 +1070,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
+      <c r="B1" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="40"/>
+      <c r="C1" s="32"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -1052,10 +1085,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="40" t="s">
+      <c r="B2" s="32" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="40"/>
+      <c r="C2" s="32"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1067,10 +1100,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="40" t="s">
+      <c r="B3" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="40"/>
+      <c r="C3" s="32"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -1082,12 +1115,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="33" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="43"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="35"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1110,7 +1143,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="32">
+      <c r="B6" s="36">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -1125,7 +1158,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="33"/>
+      <c r="B7" s="37"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -1138,7 +1171,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="33"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1151,14 +1184,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="33"/>
+      <c r="B9" s="37"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="34"/>
+      <c r="B10" s="38"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1167,16 +1200,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="35"/>
-      <c r="C11" s="36"/>
-      <c r="D11" s="36"/>
-      <c r="E11" s="37"/>
+      <c r="B11" s="39"/>
+      <c r="C11" s="40"/>
+      <c r="D11" s="40"/>
+      <c r="E11" s="41"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="32">
+      <c r="B12" s="36">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1192,7 +1225,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="33"/>
+      <c r="B13" s="37"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1205,7 +1238,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="33"/>
+      <c r="B14" s="37"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1221,7 +1254,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="33"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1236,7 +1269,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="33"/>
+      <c r="B16" s="37"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1249,7 +1282,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="33"/>
+      <c r="B17" s="37"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1260,7 +1293,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="34"/>
+      <c r="B18" s="38"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1269,16 +1302,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="35"/>
-      <c r="C19" s="36"/>
-      <c r="D19" s="36"/>
-      <c r="E19" s="37"/>
+      <c r="B19" s="39"/>
+      <c r="C19" s="40"/>
+      <c r="D19" s="40"/>
+      <c r="E19" s="41"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="32">
+      <c r="B20" s="36">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1293,7 +1326,7 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="33"/>
+      <c r="B21" s="37"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1305,7 +1338,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="33"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="8">
         <v>20</v>
       </c>
@@ -1317,7 +1350,7 @@
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="33"/>
+      <c r="B23" s="37"/>
       <c r="C23" s="8">
         <v>30</v>
       </c>
@@ -1329,7 +1362,7 @@
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="34"/>
+      <c r="B24" s="38"/>
       <c r="C24" s="10">
         <v>60</v>
       </c>
@@ -1341,16 +1374,16 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="35"/>
-      <c r="C25" s="36"/>
-      <c r="D25" s="36"/>
-      <c r="E25" s="37"/>
+      <c r="B25" s="39"/>
+      <c r="C25" s="40"/>
+      <c r="D25" s="40"/>
+      <c r="E25" s="41"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="32">
+      <c r="B26" s="36">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1368,7 +1401,7 @@
       <c r="A27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="33"/>
+      <c r="B27" s="37"/>
       <c r="C27" s="27">
         <v>20</v>
       </c>
@@ -1380,7 +1413,7 @@
       <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="33"/>
+      <c r="B28" s="37"/>
       <c r="C28" s="27">
         <v>20</v>
       </c>
@@ -1392,7 +1425,7 @@
       <c r="A29" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="33"/>
+      <c r="B29" s="37"/>
       <c r="C29" s="27">
         <v>20</v>
       </c>
@@ -1404,7 +1437,7 @@
       <c r="A30" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="33"/>
+      <c r="B30" s="37"/>
       <c r="C30" s="27">
         <v>20</v>
       </c>
@@ -1416,7 +1449,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="33"/>
+      <c r="B31" s="37"/>
       <c r="C31" s="27">
         <v>10</v>
       </c>
@@ -1428,7 +1461,7 @@
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="34"/>
+      <c r="B32" s="38"/>
       <c r="C32" s="27">
         <v>10</v>
       </c>
@@ -1441,16 +1474,16 @@
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="35"/>
-      <c r="C33" s="36"/>
-      <c r="D33" s="36"/>
-      <c r="E33" s="37"/>
+      <c r="B33" s="39"/>
+      <c r="C33" s="40"/>
+      <c r="D33" s="40"/>
+      <c r="E33" s="41"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="32">
+      <c r="B34" s="36">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1465,7 +1498,7 @@
       <c r="A35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="33"/>
+      <c r="B35" s="37"/>
       <c r="C35" s="27">
         <v>15</v>
       </c>
@@ -1477,7 +1510,7 @@
       <c r="A36" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="33"/>
+      <c r="B36" s="37"/>
       <c r="C36" s="27">
         <v>15</v>
       </c>
@@ -1490,7 +1523,7 @@
       <c r="A37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="33"/>
+      <c r="B37" s="37"/>
       <c r="C37" s="27">
         <v>30</v>
       </c>
@@ -1503,7 +1536,7 @@
       <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="33"/>
+      <c r="B38" s="37"/>
       <c r="C38" s="27">
         <v>30</v>
       </c>
@@ -1516,7 +1549,7 @@
       <c r="A39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="33"/>
+      <c r="B39" s="37"/>
       <c r="C39" s="27">
         <v>15</v>
       </c>
@@ -1529,7 +1562,7 @@
       <c r="A40" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="34"/>
+      <c r="B40" s="38"/>
       <c r="C40" s="27">
         <v>15</v>
       </c>
@@ -1539,16 +1572,16 @@
       <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="35"/>
-      <c r="C41" s="36"/>
-      <c r="D41" s="36"/>
-      <c r="E41" s="37"/>
+      <c r="B41" s="39"/>
+      <c r="C41" s="40"/>
+      <c r="D41" s="40"/>
+      <c r="E41" s="41"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="32">
+      <c r="B42" s="36">
         <f>B34+7</f>
         <v>45931</v>
       </c>
@@ -1564,7 +1597,7 @@
       <c r="A43" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="33"/>
+      <c r="B43" s="37"/>
       <c r="C43" s="8">
         <v>40</v>
       </c>
@@ -1577,7 +1610,7 @@
       <c r="A44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="33"/>
+      <c r="B44" s="37"/>
       <c r="C44" s="8">
         <v>45</v>
       </c>
@@ -1590,7 +1623,7 @@
       <c r="A45" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="33"/>
+      <c r="B45" s="37"/>
       <c r="C45" s="8">
         <v>40</v>
       </c>
@@ -1603,7 +1636,7 @@
       <c r="A46" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="33"/>
+      <c r="B46" s="37"/>
       <c r="C46" s="10">
         <v>20</v>
       </c>
@@ -1618,7 +1651,7 @@
       <c r="A47" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="34"/>
+      <c r="B47" s="38"/>
       <c r="C47" s="10">
         <v>30</v>
       </c>
@@ -1631,226 +1664,289 @@
       <c r="A48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="35"/>
-      <c r="C48" s="36"/>
-      <c r="D48" s="36"/>
-      <c r="E48" s="37"/>
+      <c r="B48" s="39"/>
+      <c r="C48" s="40"/>
+      <c r="D48" s="40"/>
+      <c r="E48" s="41"/>
     </row>
     <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A49" s="4"/>
-      <c r="B49" s="32">
+      <c r="A49" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="B49" s="36">
         <f>B42+7</f>
         <v>45938</v>
       </c>
-      <c r="C49" s="5"/>
-      <c r="D49" s="6"/>
+      <c r="C49" s="4">
+        <v>30</v>
+      </c>
+      <c r="D49" s="6" t="s">
+        <v>89</v>
+      </c>
       <c r="E49" s="5"/>
     </row>
     <row r="50" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A50" s="7"/>
-      <c r="B50" s="33"/>
-      <c r="C50" s="8"/>
-      <c r="D50" s="9"/>
+      <c r="A50" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="B50" s="37"/>
+      <c r="C50" s="7">
+        <v>30</v>
+      </c>
+      <c r="D50" s="9" t="s">
+        <v>90</v>
+      </c>
       <c r="E50" s="8"/>
     </row>
     <row r="51" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A51" s="7"/>
-      <c r="B51" s="33"/>
-      <c r="C51" s="8"/>
-      <c r="D51" s="9"/>
+      <c r="A51" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="B51" s="37"/>
+      <c r="C51" s="7">
+        <v>30</v>
+      </c>
+      <c r="D51" s="9" t="s">
+        <v>91</v>
+      </c>
       <c r="E51" s="8"/>
     </row>
     <row r="52" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A52" s="7"/>
-      <c r="B52" s="33"/>
-      <c r="C52" s="8"/>
-      <c r="D52" s="9"/>
+      <c r="A52" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="B52" s="37"/>
+      <c r="C52" s="8">
+        <v>20</v>
+      </c>
+      <c r="D52" s="9" t="s">
+        <v>93</v>
+      </c>
       <c r="E52" s="8"/>
     </row>
-    <row r="53" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A53" s="10"/>
-      <c r="B53" s="34"/>
-      <c r="C53" s="10"/>
+    <row r="53" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A53" s="23" t="s">
+        <v>96</v>
+      </c>
+      <c r="B53" s="37"/>
+      <c r="C53" s="10">
+        <v>30</v>
+      </c>
       <c r="D53" s="11"/>
       <c r="E53" s="10"/>
     </row>
-    <row r="54" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="12" t="s">
+    <row r="54" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A54" s="23" t="s">
+        <v>94</v>
+      </c>
+      <c r="B54" s="37"/>
+      <c r="C54" s="10">
+        <v>20</v>
+      </c>
+      <c r="D54" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="E54" s="10"/>
+    </row>
+    <row r="55" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A55" s="10" t="s">
+        <v>83</v>
+      </c>
+      <c r="B55" s="38"/>
+      <c r="C55" s="10">
+        <v>20</v>
+      </c>
+      <c r="D55" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="E55" s="10"/>
+    </row>
+    <row r="56" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A56" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
-      <c r="D54" s="36"/>
-      <c r="E54" s="37"/>
-    </row>
-    <row r="55" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A55" s="4"/>
-      <c r="B55" s="32">
+      <c r="B56" s="39"/>
+      <c r="C56" s="40"/>
+      <c r="D56" s="40"/>
+      <c r="E56" s="41"/>
+    </row>
+    <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="4"/>
+      <c r="B57" s="36">
         <f>B49+7</f>
         <v>45945</v>
       </c>
-      <c r="C55" s="5"/>
-      <c r="D55" s="6"/>
-      <c r="E55" s="5"/>
-    </row>
-    <row r="56" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A56" s="7"/>
-      <c r="B56" s="33"/>
-      <c r="C56" s="8"/>
-      <c r="D56" s="9"/>
-      <c r="E56" s="8"/>
-    </row>
-    <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A57" s="7"/>
-      <c r="B57" s="33"/>
-      <c r="C57" s="8"/>
-      <c r="D57" s="9"/>
-      <c r="E57" s="8"/>
+      <c r="C57" s="5"/>
+      <c r="D57" s="6"/>
+      <c r="E57" s="5"/>
     </row>
     <row r="58" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A58" s="7"/>
-      <c r="B58" s="33"/>
+      <c r="B58" s="37"/>
       <c r="C58" s="8"/>
       <c r="D58" s="9"/>
       <c r="E58" s="8"/>
     </row>
-    <row r="59" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="10"/>
-      <c r="B59" s="34"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="11"/>
-      <c r="E59" s="10"/>
-    </row>
-    <row r="60" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A60" s="12" t="s">
+    <row r="59" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="7"/>
+      <c r="B59" s="37"/>
+      <c r="C59" s="8"/>
+      <c r="D59" s="9"/>
+      <c r="E59" s="8"/>
+    </row>
+    <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A60" s="7"/>
+      <c r="B60" s="37"/>
+      <c r="C60" s="8"/>
+      <c r="D60" s="9"/>
+      <c r="E60" s="8"/>
+    </row>
+    <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="10"/>
+      <c r="B61" s="38"/>
+      <c r="C61" s="10"/>
+      <c r="D61" s="11"/>
+      <c r="E61" s="10"/>
+    </row>
+    <row r="62" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A62" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B60" s="35"/>
-      <c r="C60" s="36"/>
-      <c r="D60" s="36"/>
-      <c r="E60" s="37"/>
-    </row>
-    <row r="61" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A61" s="4"/>
-      <c r="B61" s="32">
-        <f>B55+7</f>
+      <c r="B62" s="39"/>
+      <c r="C62" s="40"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="41"/>
+    </row>
+    <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="4"/>
+      <c r="B63" s="36">
+        <f>B57+7</f>
         <v>45952</v>
       </c>
-      <c r="C61" s="5"/>
-      <c r="D61" s="6"/>
-      <c r="E61" s="5"/>
-    </row>
-    <row r="62" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="7"/>
-      <c r="B62" s="33"/>
-      <c r="C62" s="8"/>
-      <c r="D62" s="9"/>
-      <c r="E62" s="8"/>
-    </row>
-    <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="7"/>
-      <c r="B63" s="33"/>
-      <c r="C63" s="8"/>
-      <c r="D63" s="9"/>
-      <c r="E63" s="8"/>
+      <c r="C63" s="5"/>
+      <c r="D63" s="6"/>
+      <c r="E63" s="5"/>
     </row>
     <row r="64" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A64" s="7"/>
-      <c r="B64" s="33"/>
+      <c r="B64" s="37"/>
       <c r="C64" s="8"/>
       <c r="D64" s="9"/>
       <c r="E64" s="8"/>
     </row>
-    <row r="65" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A65" s="10"/>
-      <c r="B65" s="34"/>
-      <c r="C65" s="10"/>
-      <c r="D65" s="11"/>
-      <c r="E65" s="10"/>
-    </row>
-    <row r="66" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A66" s="12" t="s">
+    <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="7"/>
+      <c r="B65" s="37"/>
+      <c r="C65" s="8"/>
+      <c r="D65" s="9"/>
+      <c r="E65" s="8"/>
+    </row>
+    <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="7"/>
+      <c r="B66" s="37"/>
+      <c r="C66" s="8"/>
+      <c r="D66" s="9"/>
+      <c r="E66" s="8"/>
+    </row>
+    <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A67" s="10"/>
+      <c r="B67" s="38"/>
+      <c r="C67" s="10"/>
+      <c r="D67" s="11"/>
+      <c r="E67" s="10"/>
+    </row>
+    <row r="68" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A68" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B66" s="35"/>
-      <c r="C66" s="36"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="37"/>
-    </row>
-    <row r="67" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="13"/>
-      <c r="B67" s="32">
-        <f>B61+7</f>
+      <c r="B68" s="39"/>
+      <c r="C68" s="40"/>
+      <c r="D68" s="40"/>
+      <c r="E68" s="41"/>
+    </row>
+    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="13"/>
+      <c r="B69" s="36">
+        <f>B63+7</f>
         <v>45959</v>
       </c>
-      <c r="C67" s="13"/>
-      <c r="D67" s="14"/>
-      <c r="E67" s="13"/>
-    </row>
-    <row r="68" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="8"/>
-      <c r="B68" s="33"/>
-      <c r="C68" s="8"/>
-      <c r="D68" s="9"/>
-      <c r="E68" s="8"/>
-    </row>
-    <row r="69" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A69" s="8"/>
-      <c r="B69" s="33"/>
-      <c r="C69" s="8"/>
-      <c r="D69" s="9"/>
-      <c r="E69" s="8"/>
+      <c r="C69" s="13"/>
+      <c r="D69" s="14"/>
+      <c r="E69" s="13"/>
     </row>
     <row r="70" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A70" s="8"/>
-      <c r="B70" s="33"/>
+      <c r="B70" s="37"/>
       <c r="C70" s="8"/>
       <c r="D70" s="9"/>
       <c r="E70" s="8"/>
     </row>
-    <row r="71" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A71" s="8"/>
-      <c r="B71" s="34"/>
+      <c r="B71" s="37"/>
       <c r="C71" s="8"/>
       <c r="D71" s="9"/>
       <c r="E71" s="8"/>
     </row>
-    <row r="72" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A72" s="12" t="s">
+    <row r="72" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A72" s="8"/>
+      <c r="B72" s="37"/>
+      <c r="C72" s="8"/>
+      <c r="D72" s="9"/>
+      <c r="E72" s="8"/>
+    </row>
+    <row r="73" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A73" s="8"/>
+      <c r="B73" s="38"/>
+      <c r="C73" s="8"/>
+      <c r="D73" s="9"/>
+      <c r="E73" s="8"/>
+    </row>
+    <row r="74" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B72" s="35"/>
-      <c r="C72" s="36"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="37"/>
-    </row>
-    <row r="73" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="38" t="s">
+      <c r="B74" s="39"/>
+      <c r="C74" s="40"/>
+      <c r="D74" s="40"/>
+      <c r="E74" s="41"/>
+    </row>
+    <row r="75" spans="1:5" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A75" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="B73" s="39"/>
-      <c r="C73" s="15">
-        <f>MROUND(SUM(C6:C72) /60,0.2)</f>
-        <v>17.600000000000001</v>
-      </c>
-      <c r="D73" s="16"/>
-      <c r="E73" s="17"/>
-    </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A75" s="18" t="s">
+      <c r="B75" s="43"/>
+      <c r="C75" s="15">
+        <f>MROUND(SUM(C6:C74) /60,0.2)</f>
+        <v>20.6</v>
+      </c>
+      <c r="D75" s="16"/>
+      <c r="E75" s="17"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A77" s="18" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A76" s="18"/>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A78" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="25">
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="A75:B75"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:B67"/>
+    <mergeCell ref="B68:E68"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
     <mergeCell ref="B4:E4"/>
-    <mergeCell ref="B67:B71"/>
+    <mergeCell ref="B69:B73"/>
     <mergeCell ref="B48:E48"/>
     <mergeCell ref="B6:B10"/>
     <mergeCell ref="B11:E11"/>
@@ -1862,21 +1958,12 @@
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:B40"/>
     <mergeCell ref="B41:E41"/>
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="B72:E72"/>
-    <mergeCell ref="A73:B73"/>
-    <mergeCell ref="B49:B53"/>
-    <mergeCell ref="B54:E54"/>
-    <mergeCell ref="B55:B59"/>
-    <mergeCell ref="B60:E60"/>
-    <mergeCell ref="B61:B65"/>
-    <mergeCell ref="B66:E66"/>
   </mergeCells>
   <dataValidations count="2">
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C61:C65 C55:C59 C42:C47 C49:C53 C20:C24 B6 C12:C18 C67:C71 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C63:C67 C57:C61 C42:C47 C49:C55 C20:C24 B6 C12:C18 C69:C73 C6:C10" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B61:B65 B20:B24 B26:B32 B34:B40 B42:B47 B49:B53 B55:B59 B67:B71" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
+    <dataValidation type="date" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="B12:B18 B63:B67 B20:B24 B26:B32 B34:B40 B42:B47 B49:B55 B57:B61 B69:B73" xr:uid="{7694F886-C01B-440C-B6C8-5FF698F43C26}">
       <formula1>45261</formula1>
     </dataValidation>
   </dataValidations>
@@ -1901,15 +1988,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2152,6 +2230,15 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2164,14 +2251,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2190,6 +2269,14 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Chore(JNR) : dernier update
</commit_message>
<xml_diff>
--- a/doc/m-planification-jnltrav.xlsx
+++ b/doc/m-planification-jnltrav.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\pb17shq\Documents\Shootmeup\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91DEFB1E-23F4-49BC-90C8-1146583BBE3C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{880B4501-FFBD-4C7D-B491-306844C0A7FC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="138" uniqueCount="117">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="139" uniqueCount="118">
   <si>
     <t>Apprenti.e</t>
   </si>
@@ -401,6 +401,9 @@
   </si>
   <si>
     <t>création des colision entre joueur et ennemis, ennemis et projectils, projectils et obstacle, projectils et joueur</t>
+  </si>
+  <si>
+    <t>Couleur taille effect et freeze</t>
   </si>
 </sst>
 </file>
@@ -755,6 +758,56 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
     </xf>
@@ -766,56 +819,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="4" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1135,10 +1138,10 @@
   <dimension ref="A1:F84"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" zoomScaleSheetLayoutView="85" workbookViewId="0">
-      <pane xSplit="3" ySplit="5" topLeftCell="D35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="3" ySplit="5" topLeftCell="D50" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="D1" sqref="D1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D50" sqref="D50"/>
+      <selection pane="bottomRight" activeCell="D73" sqref="D73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="13.5" x14ac:dyDescent="0.25"/>
@@ -1157,10 +1160,10 @@
       <c r="A1" s="21" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="46" t="s">
         <v>21</v>
       </c>
-      <c r="C1" s="33"/>
+      <c r="C1" s="46"/>
       <c r="D1" s="22" t="s">
         <v>1</v>
       </c>
@@ -1172,10 +1175,10 @@
       <c r="A2" s="21" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="46" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="33"/>
+      <c r="C2" s="46"/>
       <c r="D2" s="22" t="s">
         <v>4</v>
       </c>
@@ -1187,10 +1190,10 @@
       <c r="A3" s="21" t="s">
         <v>6</v>
       </c>
-      <c r="B3" s="33" t="s">
+      <c r="B3" s="46" t="s">
         <v>18</v>
       </c>
-      <c r="C3" s="33"/>
+      <c r="C3" s="46"/>
       <c r="D3" s="22" t="s">
         <v>7</v>
       </c>
@@ -1202,12 +1205,12 @@
       <c r="A4" s="21" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="34" t="s">
+      <c r="B4" s="47" t="s">
         <v>20</v>
       </c>
-      <c r="C4" s="35"/>
-      <c r="D4" s="35"/>
-      <c r="E4" s="36"/>
+      <c r="C4" s="48"/>
+      <c r="D4" s="48"/>
+      <c r="E4" s="49"/>
     </row>
     <row r="5" spans="1:6" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A5" s="2" t="s">
@@ -1230,7 +1233,7 @@
       <c r="A6" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="37">
+      <c r="B6" s="33">
         <v>45896</v>
       </c>
       <c r="C6" s="5">
@@ -1245,7 +1248,7 @@
       <c r="A7" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="B7" s="38"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="8">
         <v>45</v>
       </c>
@@ -1258,7 +1261,7 @@
       <c r="A8" s="7" t="s">
         <v>23</v>
       </c>
-      <c r="B8" s="38"/>
+      <c r="B8" s="34"/>
       <c r="C8" s="8">
         <v>45</v>
       </c>
@@ -1271,14 +1274,14 @@
     </row>
     <row r="9" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="7"/>
-      <c r="B9" s="38"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="8"/>
       <c r="D9" s="9"/>
       <c r="E9" s="8"/>
     </row>
     <row r="10" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="10"/>
-      <c r="B10" s="39"/>
+      <c r="B10" s="35"/>
       <c r="C10" s="10"/>
       <c r="D10" s="11"/>
       <c r="E10" s="10"/>
@@ -1287,16 +1290,16 @@
       <c r="A11" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B11" s="40"/>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="42"/>
+      <c r="B11" s="36"/>
+      <c r="C11" s="37"/>
+      <c r="D11" s="37"/>
+      <c r="E11" s="38"/>
     </row>
     <row r="12" spans="1:6" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="B12" s="37">
+      <c r="B12" s="33">
         <f>B6+7</f>
         <v>45903</v>
       </c>
@@ -1312,7 +1315,7 @@
       <c r="A13" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="B13" s="38"/>
+      <c r="B13" s="34"/>
       <c r="C13" s="8">
         <v>5</v>
       </c>
@@ -1325,7 +1328,7 @@
       <c r="A14" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B14" s="38"/>
+      <c r="B14" s="34"/>
       <c r="C14" s="8">
         <v>100</v>
       </c>
@@ -1341,7 +1344,7 @@
       <c r="A15" s="7" t="s">
         <v>27</v>
       </c>
-      <c r="B15" s="38"/>
+      <c r="B15" s="34"/>
       <c r="C15" s="8">
         <v>40</v>
       </c>
@@ -1356,7 +1359,7 @@
       <c r="A16" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B16" s="38"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="10">
         <v>5</v>
       </c>
@@ -1369,7 +1372,7 @@
       <c r="A17" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B17" s="38"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="10">
         <v>5</v>
       </c>
@@ -1380,7 +1383,7 @@
     </row>
     <row r="18" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A18" s="10"/>
-      <c r="B18" s="39"/>
+      <c r="B18" s="35"/>
       <c r="C18" s="10"/>
       <c r="D18" s="11"/>
       <c r="E18" s="10"/>
@@ -1389,16 +1392,16 @@
       <c r="A19" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B19" s="40"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="42"/>
+      <c r="B19" s="36"/>
+      <c r="C19" s="37"/>
+      <c r="D19" s="37"/>
+      <c r="E19" s="38"/>
     </row>
     <row r="20" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
         <v>41</v>
       </c>
-      <c r="B20" s="37">
+      <c r="B20" s="33">
         <f>B12+7</f>
         <v>45910</v>
       </c>
@@ -1413,7 +1416,7 @@
       <c r="A21" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="B21" s="38"/>
+      <c r="B21" s="34"/>
       <c r="C21" s="8">
         <v>30</v>
       </c>
@@ -1425,7 +1428,7 @@
       <c r="A22" s="7" t="s">
         <v>44</v>
       </c>
-      <c r="B22" s="38"/>
+      <c r="B22" s="34"/>
       <c r="C22" s="8">
         <v>20</v>
       </c>
@@ -1437,7 +1440,7 @@
       <c r="A23" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B23" s="38"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="8">
         <v>30</v>
       </c>
@@ -1449,7 +1452,7 @@
       <c r="A24" s="10" t="s">
         <v>48</v>
       </c>
-      <c r="B24" s="39"/>
+      <c r="B24" s="35"/>
       <c r="C24" s="10">
         <v>60</v>
       </c>
@@ -1461,16 +1464,16 @@
       <c r="A25" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B25" s="40"/>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="42"/>
+      <c r="B25" s="36"/>
+      <c r="C25" s="37"/>
+      <c r="D25" s="37"/>
+      <c r="E25" s="38"/>
     </row>
     <row r="26" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
         <v>50</v>
       </c>
-      <c r="B26" s="37">
+      <c r="B26" s="33">
         <f>B20+7</f>
         <v>45917</v>
       </c>
@@ -1488,7 +1491,7 @@
       <c r="A27" s="7" t="s">
         <v>46</v>
       </c>
-      <c r="B27" s="38"/>
+      <c r="B27" s="34"/>
       <c r="C27" s="27">
         <v>20</v>
       </c>
@@ -1500,7 +1503,7 @@
       <c r="A28" s="7" t="s">
         <v>53</v>
       </c>
-      <c r="B28" s="38"/>
+      <c r="B28" s="34"/>
       <c r="C28" s="27">
         <v>20</v>
       </c>
@@ -1512,7 +1515,7 @@
       <c r="A29" s="27" t="s">
         <v>61</v>
       </c>
-      <c r="B29" s="38"/>
+      <c r="B29" s="34"/>
       <c r="C29" s="27">
         <v>20</v>
       </c>
@@ -1524,7 +1527,7 @@
       <c r="A30" s="23" t="s">
         <v>60</v>
       </c>
-      <c r="B30" s="38"/>
+      <c r="B30" s="34"/>
       <c r="C30" s="27">
         <v>20</v>
       </c>
@@ -1536,7 +1539,7 @@
       <c r="A31" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B31" s="38"/>
+      <c r="B31" s="34"/>
       <c r="C31" s="27">
         <v>10</v>
       </c>
@@ -1548,7 +1551,7 @@
       <c r="A32" s="7" t="s">
         <v>55</v>
       </c>
-      <c r="B32" s="39"/>
+      <c r="B32" s="35"/>
       <c r="C32" s="27">
         <v>10</v>
       </c>
@@ -1561,16 +1564,16 @@
       <c r="A33" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B33" s="40"/>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="42"/>
+      <c r="B33" s="36"/>
+      <c r="C33" s="37"/>
+      <c r="D33" s="37"/>
+      <c r="E33" s="38"/>
     </row>
     <row r="34" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A34" s="13" t="s">
         <v>63</v>
       </c>
-      <c r="B34" s="37">
+      <c r="B34" s="33">
         <f>B26+7</f>
         <v>45924</v>
       </c>
@@ -1585,7 +1588,7 @@
       <c r="A35" s="8" t="s">
         <v>66</v>
       </c>
-      <c r="B35" s="38"/>
+      <c r="B35" s="34"/>
       <c r="C35" s="27">
         <v>15</v>
       </c>
@@ -1597,7 +1600,7 @@
       <c r="A36" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B36" s="38"/>
+      <c r="B36" s="34"/>
       <c r="C36" s="27">
         <v>15</v>
       </c>
@@ -1610,7 +1613,7 @@
       <c r="A37" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B37" s="38"/>
+      <c r="B37" s="34"/>
       <c r="C37" s="27">
         <v>30</v>
       </c>
@@ -1623,7 +1626,7 @@
       <c r="A38" s="8" t="s">
         <v>72</v>
       </c>
-      <c r="B38" s="38"/>
+      <c r="B38" s="34"/>
       <c r="C38" s="27">
         <v>30</v>
       </c>
@@ -1636,7 +1639,7 @@
       <c r="A39" s="8" t="s">
         <v>69</v>
       </c>
-      <c r="B39" s="38"/>
+      <c r="B39" s="34"/>
       <c r="C39" s="27">
         <v>15</v>
       </c>
@@ -1649,7 +1652,7 @@
       <c r="A40" s="8" t="s">
         <v>71</v>
       </c>
-      <c r="B40" s="39"/>
+      <c r="B40" s="35"/>
       <c r="C40" s="27">
         <v>15</v>
       </c>
@@ -1659,16 +1662,16 @@
       <c r="A41" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B41" s="40"/>
-      <c r="C41" s="41"/>
-      <c r="D41" s="41"/>
-      <c r="E41" s="42"/>
+      <c r="B41" s="36"/>
+      <c r="C41" s="37"/>
+      <c r="D41" s="37"/>
+      <c r="E41" s="38"/>
     </row>
     <row r="42" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A42" s="4" t="s">
         <v>76</v>
       </c>
-      <c r="B42" s="37">
+      <c r="B42" s="33">
         <f>B34+7</f>
         <v>45931</v>
       </c>
@@ -1684,7 +1687,7 @@
       <c r="A43" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B43" s="38"/>
+      <c r="B43" s="34"/>
       <c r="C43" s="8">
         <v>40</v>
       </c>
@@ -1697,7 +1700,7 @@
       <c r="A44" s="7" t="s">
         <v>77</v>
       </c>
-      <c r="B44" s="38"/>
+      <c r="B44" s="34"/>
       <c r="C44" s="8">
         <v>45</v>
       </c>
@@ -1710,7 +1713,7 @@
       <c r="A45" s="7" t="s">
         <v>80</v>
       </c>
-      <c r="B45" s="38"/>
+      <c r="B45" s="34"/>
       <c r="C45" s="8">
         <v>40</v>
       </c>
@@ -1723,7 +1726,7 @@
       <c r="A46" s="23" t="s">
         <v>84</v>
       </c>
-      <c r="B46" s="38"/>
+      <c r="B46" s="34"/>
       <c r="C46" s="10">
         <v>20</v>
       </c>
@@ -1738,7 +1741,7 @@
       <c r="A47" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B47" s="39"/>
+      <c r="B47" s="35"/>
       <c r="C47" s="10">
         <v>30</v>
       </c>
@@ -1751,16 +1754,16 @@
       <c r="A48" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B48" s="40"/>
-      <c r="C48" s="41"/>
-      <c r="D48" s="41"/>
-      <c r="E48" s="42"/>
+      <c r="B48" s="36"/>
+      <c r="C48" s="37"/>
+      <c r="D48" s="37"/>
+      <c r="E48" s="38"/>
     </row>
     <row r="49" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
         <v>76</v>
       </c>
-      <c r="B49" s="37">
+      <c r="B49" s="33">
         <f>B42+7</f>
         <v>45938</v>
       </c>
@@ -1776,7 +1779,7 @@
       <c r="A50" s="1" t="s">
         <v>87</v>
       </c>
-      <c r="B50" s="38"/>
+      <c r="B50" s="34"/>
       <c r="C50" s="7">
         <v>30</v>
       </c>
@@ -1789,7 +1792,7 @@
       <c r="A51" s="1" t="s">
         <v>88</v>
       </c>
-      <c r="B51" s="38"/>
+      <c r="B51" s="34"/>
       <c r="C51" s="7">
         <v>30</v>
       </c>
@@ -1802,7 +1805,7 @@
       <c r="A52" s="7" t="s">
         <v>115</v>
       </c>
-      <c r="B52" s="38"/>
+      <c r="B52" s="34"/>
       <c r="C52" s="8">
         <v>20</v>
       </c>
@@ -1815,7 +1818,7 @@
       <c r="A53" s="23" t="s">
         <v>94</v>
       </c>
-      <c r="B53" s="38"/>
+      <c r="B53" s="34"/>
       <c r="C53" s="10">
         <v>30</v>
       </c>
@@ -1828,7 +1831,7 @@
       <c r="A54" s="23" t="s">
         <v>92</v>
       </c>
-      <c r="B54" s="38"/>
+      <c r="B54" s="34"/>
       <c r="C54" s="10">
         <v>20</v>
       </c>
@@ -1841,7 +1844,7 @@
       <c r="A55" s="10" t="s">
         <v>83</v>
       </c>
-      <c r="B55" s="39"/>
+      <c r="B55" s="35"/>
       <c r="C55" s="10">
         <v>20</v>
       </c>
@@ -1854,18 +1857,18 @@
       <c r="A56" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B56" s="45" t="s">
+      <c r="B56" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="C56" s="46"/>
-      <c r="D56" s="46"/>
-      <c r="E56" s="47"/>
+      <c r="C56" s="42"/>
+      <c r="D56" s="42"/>
+      <c r="E56" s="43"/>
     </row>
     <row r="57" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A57" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="B57" s="37">
+      <c r="B57" s="33">
         <v>45954</v>
       </c>
       <c r="C57" s="5">
@@ -1880,7 +1883,7 @@
       <c r="A58" s="7" t="s">
         <v>99</v>
       </c>
-      <c r="B58" s="48"/>
+      <c r="B58" s="44"/>
       <c r="C58" s="8">
         <v>5</v>
       </c>
@@ -1893,7 +1896,7 @@
       <c r="A59" s="7" t="s">
         <v>101</v>
       </c>
-      <c r="B59" s="48"/>
+      <c r="B59" s="44"/>
       <c r="C59" s="8">
         <v>1</v>
       </c>
@@ -1904,14 +1907,14 @@
     </row>
     <row r="60" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A60" s="7"/>
-      <c r="B60" s="48"/>
+      <c r="B60" s="44"/>
       <c r="C60" s="8"/>
       <c r="D60" s="9"/>
       <c r="E60" s="8"/>
     </row>
     <row r="61" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A61" s="10"/>
-      <c r="B61" s="49"/>
+      <c r="B61" s="45"/>
       <c r="C61" s="10"/>
       <c r="D61" s="11"/>
       <c r="E61" s="10"/>
@@ -1920,18 +1923,18 @@
       <c r="A62" s="32" t="s">
         <v>14</v>
       </c>
-      <c r="B62" s="45" t="s">
+      <c r="B62" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="C62" s="46"/>
-      <c r="D62" s="46"/>
-      <c r="E62" s="47"/>
+      <c r="C62" s="42"/>
+      <c r="D62" s="42"/>
+      <c r="E62" s="43"/>
     </row>
     <row r="63" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A63" s="4" t="s">
         <v>102</v>
       </c>
-      <c r="B63" s="37">
+      <c r="B63" s="33">
         <v>45958</v>
       </c>
       <c r="C63" s="5">
@@ -1946,7 +1949,7 @@
       <c r="A64" s="7" t="s">
         <v>103</v>
       </c>
-      <c r="B64" s="48"/>
+      <c r="B64" s="44"/>
       <c r="C64" s="8">
         <v>5</v>
       </c>
@@ -1957,21 +1960,21 @@
     </row>
     <row r="65" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A65" s="7"/>
-      <c r="B65" s="48"/>
+      <c r="B65" s="44"/>
       <c r="C65" s="8"/>
       <c r="D65" s="9"/>
       <c r="E65" s="8"/>
     </row>
     <row r="66" spans="1:5" ht="18" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A66" s="7"/>
-      <c r="B66" s="48"/>
+      <c r="B66" s="44"/>
       <c r="C66" s="8"/>
       <c r="D66" s="9"/>
       <c r="E66" s="8"/>
     </row>
     <row r="67" spans="1:5" ht="18" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A67" s="10"/>
-      <c r="B67" s="49"/>
+      <c r="B67" s="45"/>
       <c r="C67" s="10"/>
       <c r="D67" s="11"/>
       <c r="E67" s="10"/>
@@ -1980,16 +1983,16 @@
       <c r="A68" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B68" s="40"/>
-      <c r="C68" s="41"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="42"/>
+      <c r="B68" s="36"/>
+      <c r="C68" s="37"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="38"/>
     </row>
     <row r="69" spans="1:5" ht="21" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A69" s="4" t="s">
         <v>106</v>
       </c>
-      <c r="B69" s="37">
+      <c r="B69" s="33">
         <f>B49+21</f>
         <v>45959</v>
       </c>
@@ -2005,7 +2008,7 @@
       <c r="A70" s="7" t="s">
         <v>91</v>
       </c>
-      <c r="B70" s="38"/>
+      <c r="B70" s="34"/>
       <c r="C70" s="8">
         <v>30</v>
       </c>
@@ -2018,7 +2021,7 @@
       <c r="A71" s="7" t="s">
         <v>107</v>
       </c>
-      <c r="B71" s="38"/>
+      <c r="B71" s="34"/>
       <c r="C71" s="8">
         <v>20</v>
       </c>
@@ -2031,7 +2034,7 @@
       <c r="A72" s="7" t="s">
         <v>108</v>
       </c>
-      <c r="B72" s="38"/>
+      <c r="B72" s="34"/>
       <c r="C72" s="8">
         <v>10</v>
       </c>
@@ -2042,25 +2045,27 @@
       <c r="A73" s="10" t="s">
         <v>109</v>
       </c>
-      <c r="B73" s="39"/>
+      <c r="B73" s="35"/>
       <c r="C73" s="10">
         <v>30</v>
       </c>
-      <c r="D73" s="11"/>
+      <c r="D73" s="11" t="s">
+        <v>117</v>
+      </c>
       <c r="E73" s="10"/>
     </row>
     <row r="74" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A74" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B74" s="40"/>
-      <c r="C74" s="41"/>
-      <c r="D74" s="41"/>
-      <c r="E74" s="42"/>
+      <c r="B74" s="36"/>
+      <c r="C74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="38"/>
     </row>
     <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="13"/>
-      <c r="B75" s="37">
+      <c r="B75" s="33">
         <f>B69+7</f>
         <v>45966</v>
       </c>
@@ -2070,28 +2075,28 @@
     </row>
     <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="8"/>
-      <c r="B76" s="38"/>
+      <c r="B76" s="34"/>
       <c r="C76" s="8"/>
       <c r="D76" s="9"/>
       <c r="E76" s="8"/>
     </row>
     <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="8"/>
-      <c r="B77" s="38"/>
+      <c r="B77" s="34"/>
       <c r="C77" s="8"/>
       <c r="D77" s="9"/>
       <c r="E77" s="8"/>
     </row>
     <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="8"/>
-      <c r="B78" s="38"/>
+      <c r="B78" s="34"/>
       <c r="C78" s="8"/>
       <c r="D78" s="9"/>
       <c r="E78" s="8"/>
     </row>
     <row r="79" spans="1:5" ht="14.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A79" s="8"/>
-      <c r="B79" s="39"/>
+      <c r="B79" s="35"/>
       <c r="C79" s="8"/>
       <c r="D79" s="9"/>
       <c r="E79" s="8"/>
@@ -2100,16 +2105,16 @@
       <c r="A80" s="12" t="s">
         <v>14</v>
       </c>
-      <c r="B80" s="40"/>
-      <c r="C80" s="41"/>
-      <c r="D80" s="41"/>
-      <c r="E80" s="42"/>
+      <c r="B80" s="36"/>
+      <c r="C80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="38"/>
     </row>
     <row r="81" spans="1:5" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A81" s="43" t="s">
+      <c r="A81" s="39" t="s">
         <v>15</v>
       </c>
-      <c r="B81" s="44"/>
+      <c r="B81" s="40"/>
       <c r="C81" s="15">
         <f>MROUND(SUM(C6:C80) /60,0.2)</f>
         <v>23.6</v>
@@ -2127,17 +2132,6 @@
     </row>
   </sheetData>
   <mergeCells count="27">
-    <mergeCell ref="B42:B47"/>
-    <mergeCell ref="B80:E80"/>
-    <mergeCell ref="A81:B81"/>
-    <mergeCell ref="B49:B55"/>
-    <mergeCell ref="B68:E68"/>
-    <mergeCell ref="B69:B73"/>
-    <mergeCell ref="B74:E74"/>
-    <mergeCell ref="B56:E56"/>
-    <mergeCell ref="B57:B61"/>
-    <mergeCell ref="B62:E62"/>
-    <mergeCell ref="B63:B67"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B2:C2"/>
     <mergeCell ref="B3:C3"/>
@@ -2154,6 +2148,17 @@
     <mergeCell ref="B33:E33"/>
     <mergeCell ref="B34:B40"/>
     <mergeCell ref="B41:E41"/>
+    <mergeCell ref="B42:B47"/>
+    <mergeCell ref="B80:E80"/>
+    <mergeCell ref="A81:B81"/>
+    <mergeCell ref="B49:B55"/>
+    <mergeCell ref="B68:E68"/>
+    <mergeCell ref="B69:B73"/>
+    <mergeCell ref="B74:E74"/>
+    <mergeCell ref="B56:E56"/>
+    <mergeCell ref="B57:B61"/>
+    <mergeCell ref="B62:E62"/>
+    <mergeCell ref="B63:B67"/>
   </mergeCells>
   <dataValidations count="2">
     <dataValidation type="whole" operator="greaterThan" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Durée par tranche de 10min" error="Le nombre doit être de type entier" sqref="C69:C73 C42:C47 C20:C24 B6 C12:C18 C75:C79 C6:C10 C49:C55 C57:C61 C63:C67" xr:uid="{345ABA8F-B69F-4AFC-9D0E-D2AB0ACDE277}">
@@ -2184,6 +2189,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101005A5B8F5EAAC22C48A11F5D9A60E6F21D" ma:contentTypeVersion="16" ma:contentTypeDescription="Crée un document." ma:contentTypeScope="" ma:versionID="f2b963976306cc54294b7f4545a3c6c4">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="a1b10758-7132-46a4-a2fe-7a2cf46f51f4" xmlns:ns3="f7d9f5a6-831d-4621-8c77-cbcaf993e406" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="e5e135fa2fc1295e1586ddcd9c1a8904" ns2:_="" ns3:_="">
     <xsd:import namespace="a1b10758-7132-46a4-a2fe-7a2cf46f51f4"/>
@@ -2426,15 +2440,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
@@ -2447,6 +2452,14 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{40597E6F-FA73-4A07-893F-099FDC15B64D}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2465,14 +2478,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{38BCAAC0-9C03-42D2-8685-2E30F60CCBAA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{0E6F7E92-72FE-4C94-B42F-AE9EA593DE95}">
   <ds:schemaRefs>

</xml_diff>